<commit_message>
-update templates for csi and TH and formatting -New user management
</commit_message>
<xml_diff>
--- a/data-raw/TH CSI template.xlsx
+++ b/data-raw/TH CSI template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/07c4d937b78de3ca/IMPROVAST/ACS/CSIemail/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="162" documentId="8_{40006AFF-42AF-48C0-A0C6-18249D646B6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2E0ECE6F-44F6-4C50-A8DF-5CC3E211276A}"/>
+  <xr:revisionPtr revIDLastSave="168" documentId="8_{40006AFF-42AF-48C0-A0C6-18249D646B6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1ECA4DEF-AE1A-48BE-A723-311D914CD04F}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CSI" sheetId="1" r:id="rId1"/>
@@ -451,40 +451,39 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.28515625" customWidth="1"/>
-    <col min="2" max="2" width="7.85546875" customWidth="1"/>
+    <col min="2" max="2" width="14" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" customWidth="1"/>
-    <col min="5" max="5" width="31.85546875" customWidth="1"/>
+    <col min="4" max="4" width="31.85546875" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" customWidth="1"/>
     <col min="6" max="6" width="8" customWidth="1"/>
     <col min="7" max="7" width="8.42578125" customWidth="1"/>
-    <col min="8" max="8" width="10.42578125" customWidth="1"/>
-    <col min="9" max="9" width="11.28515625" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D1" s="8" t="s">
         <v>6</v>
       </c>
       <c r="E1" s="8"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D2" s="8" t="s">
         <v>7</v>
       </c>
       <c r="E2" s="8"/>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -492,9 +491,8 @@
       <c r="C3" s="9"/>
       <c r="D3" s="2"/>
       <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
@@ -502,12 +500,11 @@
       <c r="C4" s="10"/>
       <c r="D4" s="2"/>
       <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>1</v>
       </c>
@@ -516,7 +513,7 @@
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>3</v>
       </c>
@@ -525,10 +522,10 @@
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>0</v>
       </c>
@@ -536,7 +533,7 @@
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>5</v>
       </c>
@@ -544,7 +541,7 @@
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
     </row>
-    <row r="11" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="6"/>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
@@ -552,9 +549,8 @@
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-    </row>
-    <row r="12" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    </row>
+    <row r="12" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="D1:E1"/>
@@ -566,6 +562,6 @@
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="88" fitToHeight="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="92" fitToHeight="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>